<commit_message>
Update simulation case 9 files
</commit_message>
<xml_diff>
--- a/SimulationStudyData/Model2/SimCase9_zsim_SimRun1.xlsx
+++ b/SimulationStudyData/Model2/SimCase9_zsim_SimRun1.xlsx
@@ -358,7 +358,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -373,12 +373,12 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -413,12 +413,12 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -428,7 +428,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -438,22 +438,22 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -463,7 +463,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -478,12 +478,12 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -503,7 +503,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -513,27 +513,27 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -543,17 +543,17 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -563,12 +563,12 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -588,17 +588,17 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
@@ -613,17 +613,17 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -633,7 +633,7 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -643,7 +643,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -653,12 +653,12 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -668,7 +668,7 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -678,12 +678,12 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -698,7 +698,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -723,17 +723,17 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -758,22 +758,22 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87">
@@ -783,7 +783,7 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -798,12 +798,12 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -813,12 +813,12 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -863,12 +863,12 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
@@ -878,17 +878,17 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110">
@@ -898,7 +898,7 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -923,7 +923,7 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -938,7 +938,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -963,7 +963,7 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125">
@@ -973,22 +973,22 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -998,7 +998,7 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
@@ -1013,7 +1013,7 @@
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -1023,7 +1023,7 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
@@ -1043,7 +1043,7 @@
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141">
@@ -1068,22 +1068,22 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -1098,12 +1098,12 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -1113,22 +1113,22 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
@@ -1138,7 +1138,7 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -1148,7 +1148,7 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -1158,7 +1158,7 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -1188,7 +1188,7 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -1198,7 +1198,7 @@
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
@@ -1228,7 +1228,7 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
@@ -1243,42 +1243,42 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188">
@@ -1288,7 +1288,7 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190">
@@ -1303,12 +1303,12 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -1318,17 +1318,17 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198">
@@ -1348,7 +1348,7 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>